<commit_message>
fixed hours worked df
</commit_message>
<xml_diff>
--- a/data/Employees.xlsx
+++ b/data/Employees.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IsaacEvans\Documents\Uni\Applied_Data_Science\european_productivity\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26922365-2F2D-459C-AECE-2B9CC10066EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48B1A254-2AA2-4B41-B7C1-4DCD31740992}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4428" yWindow="3360" windowWidth="17280" windowHeight="8880" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4327" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4328" uniqueCount="168">
   <si>
     <t>Employees by sex, age and occupation (1 000) [LFSQ_EEGAIS__custom_2389654]</t>
   </si>
@@ -524,6 +524,9 @@
   <si>
     <t>d</t>
   </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
 </sst>
 </file>
 
@@ -591,7 +594,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -614,11 +617,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB0B0B0"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB0B0B0"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -676,6 +690,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2315,10 +2332,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:GK36"/>
+  <dimension ref="A1:GK37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="CB2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="A37" sqref="A37:XFD43"/>
@@ -23437,104 +23454,109 @@
         <v>162</v>
       </c>
     </row>
+    <row r="37" spans="1:193" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="21" t="s">
+        <v>167</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="96">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="R1:S1"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="V1:W1"/>
+    <mergeCell ref="X1:Y1"/>
+    <mergeCell ref="Z1:AA1"/>
+    <mergeCell ref="AB1:AC1"/>
+    <mergeCell ref="AD1:AE1"/>
+    <mergeCell ref="AF1:AG1"/>
+    <mergeCell ref="AH1:AI1"/>
+    <mergeCell ref="AJ1:AK1"/>
+    <mergeCell ref="AL1:AM1"/>
+    <mergeCell ref="AN1:AO1"/>
+    <mergeCell ref="AP1:AQ1"/>
+    <mergeCell ref="AR1:AS1"/>
+    <mergeCell ref="AT1:AU1"/>
+    <mergeCell ref="AV1:AW1"/>
+    <mergeCell ref="AX1:AY1"/>
+    <mergeCell ref="AZ1:BA1"/>
+    <mergeCell ref="BB1:BC1"/>
+    <mergeCell ref="BD1:BE1"/>
+    <mergeCell ref="BF1:BG1"/>
+    <mergeCell ref="BH1:BI1"/>
+    <mergeCell ref="BJ1:BK1"/>
+    <mergeCell ref="BL1:BM1"/>
+    <mergeCell ref="BN1:BO1"/>
+    <mergeCell ref="BP1:BQ1"/>
+    <mergeCell ref="BR1:BS1"/>
+    <mergeCell ref="BT1:BU1"/>
+    <mergeCell ref="BV1:BW1"/>
+    <mergeCell ref="BX1:BY1"/>
+    <mergeCell ref="BZ1:CA1"/>
+    <mergeCell ref="CB1:CC1"/>
+    <mergeCell ref="CD1:CE1"/>
+    <mergeCell ref="CF1:CG1"/>
+    <mergeCell ref="CH1:CI1"/>
+    <mergeCell ref="CJ1:CK1"/>
+    <mergeCell ref="CL1:CM1"/>
+    <mergeCell ref="CN1:CO1"/>
+    <mergeCell ref="CP1:CQ1"/>
+    <mergeCell ref="CR1:CS1"/>
+    <mergeCell ref="CT1:CU1"/>
+    <mergeCell ref="CV1:CW1"/>
+    <mergeCell ref="CX1:CY1"/>
+    <mergeCell ref="CZ1:DA1"/>
+    <mergeCell ref="DB1:DC1"/>
+    <mergeCell ref="DD1:DE1"/>
+    <mergeCell ref="DF1:DG1"/>
+    <mergeCell ref="DH1:DI1"/>
+    <mergeCell ref="DJ1:DK1"/>
+    <mergeCell ref="DL1:DM1"/>
+    <mergeCell ref="DN1:DO1"/>
+    <mergeCell ref="DP1:DQ1"/>
+    <mergeCell ref="DR1:DS1"/>
+    <mergeCell ref="DT1:DU1"/>
+    <mergeCell ref="DV1:DW1"/>
+    <mergeCell ref="DX1:DY1"/>
+    <mergeCell ref="DZ1:EA1"/>
+    <mergeCell ref="EB1:EC1"/>
+    <mergeCell ref="ED1:EE1"/>
+    <mergeCell ref="EF1:EG1"/>
+    <mergeCell ref="EH1:EI1"/>
+    <mergeCell ref="EJ1:EK1"/>
+    <mergeCell ref="EL1:EM1"/>
+    <mergeCell ref="EN1:EO1"/>
+    <mergeCell ref="EP1:EQ1"/>
+    <mergeCell ref="ER1:ES1"/>
+    <mergeCell ref="ET1:EU1"/>
+    <mergeCell ref="EV1:EW1"/>
+    <mergeCell ref="EX1:EY1"/>
+    <mergeCell ref="EZ1:FA1"/>
+    <mergeCell ref="FB1:FC1"/>
+    <mergeCell ref="FD1:FE1"/>
+    <mergeCell ref="FF1:FG1"/>
+    <mergeCell ref="FH1:FI1"/>
+    <mergeCell ref="FJ1:FK1"/>
+    <mergeCell ref="FL1:FM1"/>
+    <mergeCell ref="FN1:FO1"/>
+    <mergeCell ref="FP1:FQ1"/>
+    <mergeCell ref="FR1:FS1"/>
+    <mergeCell ref="FT1:FU1"/>
+    <mergeCell ref="FV1:FW1"/>
+    <mergeCell ref="FX1:FY1"/>
     <mergeCell ref="GJ1:GK1"/>
     <mergeCell ref="FZ1:GA1"/>
     <mergeCell ref="GB1:GC1"/>
     <mergeCell ref="GD1:GE1"/>
     <mergeCell ref="GF1:GG1"/>
     <mergeCell ref="GH1:GI1"/>
-    <mergeCell ref="FP1:FQ1"/>
-    <mergeCell ref="FR1:FS1"/>
-    <mergeCell ref="FT1:FU1"/>
-    <mergeCell ref="FV1:FW1"/>
-    <mergeCell ref="FX1:FY1"/>
-    <mergeCell ref="FF1:FG1"/>
-    <mergeCell ref="FH1:FI1"/>
-    <mergeCell ref="FJ1:FK1"/>
-    <mergeCell ref="FL1:FM1"/>
-    <mergeCell ref="FN1:FO1"/>
-    <mergeCell ref="EV1:EW1"/>
-    <mergeCell ref="EX1:EY1"/>
-    <mergeCell ref="EZ1:FA1"/>
-    <mergeCell ref="FB1:FC1"/>
-    <mergeCell ref="FD1:FE1"/>
-    <mergeCell ref="EL1:EM1"/>
-    <mergeCell ref="EN1:EO1"/>
-    <mergeCell ref="EP1:EQ1"/>
-    <mergeCell ref="ER1:ES1"/>
-    <mergeCell ref="ET1:EU1"/>
-    <mergeCell ref="EB1:EC1"/>
-    <mergeCell ref="ED1:EE1"/>
-    <mergeCell ref="EF1:EG1"/>
-    <mergeCell ref="EH1:EI1"/>
-    <mergeCell ref="EJ1:EK1"/>
-    <mergeCell ref="DR1:DS1"/>
-    <mergeCell ref="DT1:DU1"/>
-    <mergeCell ref="DV1:DW1"/>
-    <mergeCell ref="DX1:DY1"/>
-    <mergeCell ref="DZ1:EA1"/>
-    <mergeCell ref="DH1:DI1"/>
-    <mergeCell ref="DJ1:DK1"/>
-    <mergeCell ref="DL1:DM1"/>
-    <mergeCell ref="DN1:DO1"/>
-    <mergeCell ref="DP1:DQ1"/>
-    <mergeCell ref="CX1:CY1"/>
-    <mergeCell ref="CZ1:DA1"/>
-    <mergeCell ref="DB1:DC1"/>
-    <mergeCell ref="DD1:DE1"/>
-    <mergeCell ref="DF1:DG1"/>
-    <mergeCell ref="CN1:CO1"/>
-    <mergeCell ref="CP1:CQ1"/>
-    <mergeCell ref="CR1:CS1"/>
-    <mergeCell ref="CT1:CU1"/>
-    <mergeCell ref="CV1:CW1"/>
-    <mergeCell ref="CD1:CE1"/>
-    <mergeCell ref="CF1:CG1"/>
-    <mergeCell ref="CH1:CI1"/>
-    <mergeCell ref="CJ1:CK1"/>
-    <mergeCell ref="CL1:CM1"/>
-    <mergeCell ref="BT1:BU1"/>
-    <mergeCell ref="BV1:BW1"/>
-    <mergeCell ref="BX1:BY1"/>
-    <mergeCell ref="BZ1:CA1"/>
-    <mergeCell ref="CB1:CC1"/>
-    <mergeCell ref="BJ1:BK1"/>
-    <mergeCell ref="BL1:BM1"/>
-    <mergeCell ref="BN1:BO1"/>
-    <mergeCell ref="BP1:BQ1"/>
-    <mergeCell ref="BR1:BS1"/>
-    <mergeCell ref="AZ1:BA1"/>
-    <mergeCell ref="BB1:BC1"/>
-    <mergeCell ref="BD1:BE1"/>
-    <mergeCell ref="BF1:BG1"/>
-    <mergeCell ref="BH1:BI1"/>
-    <mergeCell ref="AP1:AQ1"/>
-    <mergeCell ref="AR1:AS1"/>
-    <mergeCell ref="AT1:AU1"/>
-    <mergeCell ref="AV1:AW1"/>
-    <mergeCell ref="AX1:AY1"/>
-    <mergeCell ref="AF1:AG1"/>
-    <mergeCell ref="AH1:AI1"/>
-    <mergeCell ref="AJ1:AK1"/>
-    <mergeCell ref="AL1:AM1"/>
-    <mergeCell ref="AN1:AO1"/>
-    <mergeCell ref="V1:W1"/>
-    <mergeCell ref="X1:Y1"/>
-    <mergeCell ref="Z1:AA1"/>
-    <mergeCell ref="AB1:AC1"/>
-    <mergeCell ref="AD1:AE1"/>
-    <mergeCell ref="L1:M1"/>
-    <mergeCell ref="N1:O1"/>
-    <mergeCell ref="P1:Q1"/>
-    <mergeCell ref="R1:S1"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="J1:K1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>